<commit_message>
suite commentaire récap grp 4 et 5
</commit_message>
<xml_diff>
--- a/Tests/test_recap_group_4.xlsx
+++ b/Tests/test_recap_group_4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierrick Herve\Documents\Etudes\Master SID\Watchnews\Groupe10_Robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierrick Herve\Documents\Etudes\Master SID\Watchnews\Groupe10_Robot\Groupe10_Qualite_communication\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>nom fichier</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>le temps d'exécution du message s'affiche</t>
+  </si>
+  <si>
+    <t>pas de fonctions</t>
   </si>
 </sst>
 </file>
@@ -112,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -135,11 +138,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,6 +178,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,7 +468,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +512,7 @@
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -511,7 +529,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="6"/>
       <c r="C4" s="10">
         <v>43115</v>
@@ -524,7 +542,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="6"/>
       <c r="C5" s="10">
         <v>43115</v>
@@ -537,7 +555,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="6"/>
       <c r="C6" s="10">
         <v>43115</v>
@@ -550,7 +568,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="6"/>
       <c r="C7" s="10"/>
       <c r="D7" s="3" t="s">
@@ -558,7 +576,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -572,7 +590,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="6"/>
       <c r="C9" s="10"/>
       <c r="D9" t="s">
@@ -580,7 +598,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="6"/>
       <c r="C10" s="10"/>
       <c r="D10" t="s">
@@ -588,9 +606,12 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="6"/>
       <c r="C11" s="10"/>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
@@ -660,6 +681,10 @@
       <c r="B25" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
suite tests groupe 4 et 5
</commit_message>
<xml_diff>
--- a/Tests/test_recap_group_4.xlsx
+++ b/Tests/test_recap_group_4.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>nom fichier</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>parserV1.py</t>
-  </si>
-  <si>
-    <t>tester les cas qui échouent ? À priori pas possible car la fonction n'a pas de paramètres</t>
   </si>
   <si>
     <t>à tester avec des vrais données</t>
@@ -75,16 +72,24 @@
 (car pas de fonction)</t>
   </si>
   <si>
-    <t>une erreur est levée</t>
-  </si>
-  <si>
-    <t>cas nominal (aucune erreur n'est levée)</t>
-  </si>
-  <si>
-    <t>le temps d'exécution du message s'affiche</t>
-  </si>
-  <si>
-    <t>pas de fonctions</t>
+    <t>96%
+(2 warnings
+et 1 lignes de code mort
+sur 70 lignes de code)</t>
+  </si>
+  <si>
+    <t>les exceptions sont traitées (on affiche leur nom)</t>
+  </si>
+  <si>
+    <t>le message "&lt;nom_journal&gt; OK"</t>
+  </si>
+  <si>
+    <t>80%
+(25 warnings
+sur 125 lignes de code)</t>
+  </si>
+  <si>
+    <t>bug</t>
   </si>
 </sst>
 </file>
@@ -151,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,11 +184,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -468,7 +476,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +508,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -511,8 +519,8 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -527,9 +535,12 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
+      <c r="F3" s="13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="6"/>
       <c r="C4" s="10">
         <v>43115</v>
@@ -540,9 +551,10 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="6"/>
       <c r="C5" s="10">
         <v>43115</v>
@@ -551,11 +563,12 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="6"/>
       <c r="C6" s="10">
         <v>43115</v>
@@ -566,52 +579,59 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="6"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="D7" s="3"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="10">
-        <v>43115</v>
+        <v>43117</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="6"/>
       <c r="C9" s="10"/>
       <c r="D9" t="s">
         <v>17</v>
       </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="6"/>
       <c r="C10" s="10"/>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="6"/>
       <c r="C11" s="10"/>
-      <c r="D11" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="D11" s="3"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
@@ -681,9 +701,11 @@
       <c r="B25" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A8:A11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="F3:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>